<commit_message>
beräkning av kortaste väg
</commit_message>
<xml_diff>
--- a/C-kod/Karta.xlsx
+++ b/C-kod/Karta.xlsx
@@ -25,7 +25,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -41,8 +41,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -73,6 +79,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -166,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -191,6 +209,18 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:M12"/>
+  <dimension ref="B3:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +582,9 @@
       <c r="E5" s="3">
         <v>1</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="13">
+        <v>20</v>
+      </c>
       <c r="G5" s="8"/>
       <c r="H5" s="3"/>
       <c r="I5" s="8"/>
@@ -572,8 +604,10 @@
         <v>3</v>
       </c>
       <c r="E6" s="17"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="3">
+        <v>19</v>
+      </c>
+      <c r="G6" s="14"/>
       <c r="H6" s="3"/>
       <c r="I6" s="8"/>
       <c r="J6" s="3"/>
@@ -592,7 +626,9 @@
         <v>4</v>
       </c>
       <c r="E7" s="17"/>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3">
+        <v>18</v>
+      </c>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
       <c r="I7" s="8"/>
@@ -615,13 +651,13 @@
         <v>6</v>
       </c>
       <c r="F8" s="3">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="G8" s="13">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="H8" s="13">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="I8" s="17"/>
       <c r="J8" s="13"/>
@@ -647,7 +683,7 @@
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="13">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="I9" s="17"/>
       <c r="J9" s="8"/>
@@ -667,9 +703,9 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="3">
-        <v>11</v>
-      </c>
-      <c r="I10" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="I10" s="14"/>
       <c r="J10" s="3"/>
       <c r="K10" s="13"/>
       <c r="L10" s="11"/>
@@ -729,6 +765,256 @@
         <v>7</v>
       </c>
     </row>
+    <row r="16" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="15">
+        <v>16</v>
+      </c>
+      <c r="D16" s="15">
+        <v>15</v>
+      </c>
+      <c r="E16" s="16">
+        <v>14</v>
+      </c>
+      <c r="F16" s="16">
+        <v>13</v>
+      </c>
+      <c r="G16" s="16">
+        <v>12</v>
+      </c>
+      <c r="H16" s="16">
+        <v>11</v>
+      </c>
+      <c r="I16" s="16">
+        <v>10</v>
+      </c>
+      <c r="J16" s="16">
+        <v>9</v>
+      </c>
+      <c r="K16" s="16">
+        <v>8</v>
+      </c>
+      <c r="L16" s="16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="15">
+        <v>14</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="27">
+        <v>0</v>
+      </c>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="35">
+        <v>19</v>
+      </c>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="15">
+        <v>15</v>
+      </c>
+      <c r="C18" s="26"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="13">
+        <v>1</v>
+      </c>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="14">
+        <v>18</v>
+      </c>
+      <c r="I18" s="25"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="33">
+        <v>16</v>
+      </c>
+      <c r="C19" s="34">
+        <v>4</v>
+      </c>
+      <c r="D19" s="13">
+        <v>3</v>
+      </c>
+      <c r="E19" s="13">
+        <v>2</v>
+      </c>
+      <c r="F19" s="13">
+        <v>19</v>
+      </c>
+      <c r="G19" s="13">
+        <v>18</v>
+      </c>
+      <c r="H19" s="13">
+        <v>17</v>
+      </c>
+      <c r="I19" s="14"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="15">
+        <v>17</v>
+      </c>
+      <c r="C20" s="26"/>
+      <c r="D20" s="13">
+        <v>4</v>
+      </c>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="13">
+        <v>16</v>
+      </c>
+      <c r="I20" s="25"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="15">
+        <v>18</v>
+      </c>
+      <c r="C21" s="26"/>
+      <c r="D21" s="13">
+        <v>5</v>
+      </c>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="13">
+        <v>15</v>
+      </c>
+      <c r="I21" s="25"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="16">
+        <v>19</v>
+      </c>
+      <c r="C22" s="26"/>
+      <c r="D22" s="13">
+        <v>6</v>
+      </c>
+      <c r="E22" s="13">
+        <v>7</v>
+      </c>
+      <c r="F22" s="13">
+        <v>8</v>
+      </c>
+      <c r="G22" s="13">
+        <v>9</v>
+      </c>
+      <c r="H22" s="13">
+        <v>14</v>
+      </c>
+      <c r="I22" s="14"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="15">
+        <v>20</v>
+      </c>
+      <c r="C23" s="31"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="13">
+        <v>13</v>
+      </c>
+      <c r="I23" s="25"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="15">
+        <v>21</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="32">
+        <v>12</v>
+      </c>
+      <c r="I24" s="9"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C25" s="15">
+        <v>16</v>
+      </c>
+      <c r="D25" s="15">
+        <v>15</v>
+      </c>
+      <c r="E25" s="16">
+        <v>14</v>
+      </c>
+      <c r="F25" s="16">
+        <v>13</v>
+      </c>
+      <c r="G25" s="16">
+        <v>12</v>
+      </c>
+      <c r="H25" s="16">
+        <v>11</v>
+      </c>
+      <c r="I25" s="16">
+        <v>10</v>
+      </c>
+      <c r="J25" s="16">
+        <v>9</v>
+      </c>
+      <c r="K25" s="16">
+        <v>8</v>
+      </c>
+      <c r="L25" s="16">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>